<commit_message>
external eval data processing and resources
</commit_message>
<xml_diff>
--- a/resources/forms/001-market-baseline-retailers.xlsx
+++ b/resources/forms/001-market-baseline-retailers.xlsx
@@ -99,7 +99,7 @@
     <t>${Survey_Location} = 'other'</t>
   </si>
   <si>
-    <t>. = ''</t>
+    <t>. != ''</t>
   </si>
   <si>
     <t>end_group</t>
@@ -201,7 +201,7 @@
     <t>How many iron boxes does the retailer sell every month?</t>
   </si>
   <si>
-    <t>retailer_cutomer_region</t>
+    <t>retailer_customer_region</t>
   </si>
   <si>
     <t>What region does the retailer's customers usually come from?</t>
@@ -243,7 +243,7 @@
     <t>How much inventory does the retailer hold onto every month?</t>
   </si>
   <si>
-    <t>retailers_market_estimate</t>
+    <t>retailer_market_estimate</t>
   </si>
   <si>
     <t>According to the retailers, approximately how many ironing vyapaaris are there in the city?</t>
@@ -297,7 +297,7 @@
     <t>Are the retailers interested in selling LPG iron boxes?</t>
   </si>
   <si>
-    <t>reatiler_lpg_rejection</t>
+    <t>retailer_lpg_rejection</t>
   </si>
   <si>
     <t>If no, what is the reason for the retailer to not sell LPG iron boxes?</t>
@@ -324,7 +324,7 @@
     <t>__version__</t>
   </si>
   <si>
-    <t>'vErakmWpy6eg9y4s2PwsFM'</t>
+    <t>'vSDc6jKQNyUmrTchR9SySA'</t>
   </si>
   <si>
     <t>list_name</t>
@@ -423,7 +423,7 @@
     <t>Market Entry Survey and Baseline - Retailers</t>
   </si>
   <si>
-    <t>11 (2022-10-19 04:53:16)</t>
+    <t>12 (2022-11-10 09:11:38)</t>
   </si>
 </sst>
 </file>

</xml_diff>